<commit_message>
Update observation data submission form, new Data Use Release Form
</commit_message>
<xml_diff>
--- a/pages/data/template-observation-submission.xlsx
+++ b/pages/data/template-observation-submission.xlsx
@@ -1,26 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29429"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitcheka\Desktop\Websitenewstuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitcheka\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{52C76049-8D65-4DB4-AD8A-C9655D576172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58F33735-8199-4256-9BC0-0A1B9800131A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8610"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SITES" sheetId="1" r:id="rId1"/>
-    <sheet name="TAXA" sheetId="2" r:id="rId2"/>
+    <sheet name="Readme" sheetId="3" r:id="rId1"/>
+    <sheet name="Sites" sheetId="1" r:id="rId2"/>
+    <sheet name="Taxa" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+  <si>
+    <t>Thank you for submitting a site list to OregonFlora!</t>
+  </si>
+  <si>
+    <t>The taxa tab can list any number of taxa for each site, linked by a matching value in the Site Number column.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please: </t>
+  </si>
+  <si>
+    <t>&gt; Use the current nomenclature on oregonflora.org.</t>
+  </si>
+  <si>
+    <t>&gt; Choose LatLong decimal OR UTM OR Township-Range-Section-etc. for your site center.</t>
+  </si>
+  <si>
+    <t>&gt; Submit a Data Use Release form for each observer to OregonFlora. This form is available at: https://oregonflora.org/pages/data/DataUseRelease_OregonFlora.pdf</t>
+  </si>
+  <si>
+    <t>&gt; Completed workbooks may be emailed to info@oregonflora.org.</t>
+  </si>
+  <si>
+    <t>Thank you again!</t>
+  </si>
+  <si>
+    <t>the OregonFlora team</t>
+  </si>
+  <si>
+    <t>Observers (1 to many)</t>
+  </si>
+  <si>
+    <t>Observation Date</t>
+  </si>
+  <si>
+    <t>Radius</t>
+  </si>
+  <si>
+    <t>Elevation</t>
+  </si>
+  <si>
+    <t>Lat/Long Coordinates, decimal degrees</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>TRS Coordinates</t>
+  </si>
+  <si>
+    <t>UTM Coordinates</t>
+  </si>
   <si>
     <t>Site Number</t>
   </si>
@@ -37,9 +106,6 @@
     <t>Observer 3</t>
   </si>
   <si>
-    <t>Observers (1 to many)</t>
-  </si>
-  <si>
     <t>Month</t>
   </si>
   <si>
@@ -49,12 +115,33 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Observation Date</t>
-  </si>
-  <si>
     <t>County</t>
   </si>
   <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Elev. Min</t>
+  </si>
+  <si>
+    <t>Elev. Max</t>
+  </si>
+  <si>
+    <t>Elev. Unit</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>GPS accuracy</t>
+  </si>
+  <si>
     <t>Township</t>
   </si>
   <si>
@@ -70,68 +157,23 @@
     <t>1/16 Section</t>
   </si>
   <si>
-    <t>TRS Coordinates</t>
-  </si>
-  <si>
-    <t>LatDegrees</t>
-  </si>
-  <si>
-    <t>LongDegrees</t>
-  </si>
-  <si>
-    <t>Datum</t>
-  </si>
-  <si>
-    <t>GPS accuracy</t>
+    <t>UTM Northing</t>
   </si>
   <si>
     <t>UTM Easting</t>
   </si>
   <si>
-    <t>UTM Northing</t>
-  </si>
-  <si>
     <t>UTM Zone</t>
   </si>
   <si>
-    <t>UTM Coordinates</t>
-  </si>
-  <si>
-    <t>Radius</t>
-  </si>
-  <si>
     <t>Taxon</t>
-  </si>
-  <si>
-    <t>Elev. Max</t>
-  </si>
-  <si>
-    <t>Elev. Min</t>
-  </si>
-  <si>
-    <t>Elev. Unit</t>
-  </si>
-  <si>
-    <t>Lat/Long Coordinates, decimal degrees</t>
-  </si>
-  <si>
-    <t>Elevation</t>
-  </si>
-  <si>
-    <t>Latitude and Longitude Coordinates</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,12 +198,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="47"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -196,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -213,26 +249,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -241,17 +313,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -276,9 +348,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,9 +388,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -353,7 +425,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +460,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -561,194 +633,255 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118AAC64-D698-4CA6-B76A-AC152422D152}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="94.28515625" style="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30.75">
+      <c r="B3" s="21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" customHeight="1">
+      <c r="B8" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AE11"/>
+  <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="14" max="17" width="11.85546875" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" customWidth="1"/>
-    <col min="24" max="24" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8" customWidth="1"/>
-    <col min="26" max="26" width="13" customWidth="1"/>
-    <col min="27" max="27" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7" customWidth="1"/>
+    <col min="15" max="19" width="11.85546875" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="C1" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16" t="s">
+    <row r="1" spans="1:29">
+      <c r="C1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="K1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="20"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>12</v>
+      </c>
       <c r="M1" s="20"/>
-      <c r="N1" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="19"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="P1" s="19"/>
       <c r="Q1" s="19"/>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="19"/>
+      <c r="S1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="18" t="s">
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="15"/>
+    </row>
+    <row r="2" spans="1:29" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-    </row>
-    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="12" t="s">
+      <c r="R2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="S2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="V2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="M9" s="5"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="M11" s="5"/>
+      <c r="U2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="N9" s="4"/>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="N11" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="AA1:AE1"/>
+  <mergeCells count="6">
+    <mergeCell ref="Y1:AC1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="L1:N1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -756,16 +889,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" customWidth="1"/>
@@ -774,25 +907,13 @@
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+    <row r="1" spans="1:2" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>